<commit_message>
Updating Nkabom Project Files
</commit_message>
<xml_diff>
--- a/coordinators.xlsx
+++ b/coordinators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobcumulus\WebstormProjects\mcgill_nkabom_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobcumulus\WebstormProjects\cradle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2FC83C-8DF7-4100-BE5C-A198EBC4E386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CC7C1C-57DB-4C75-BA1C-538EE57CA5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>firstName</t>
   </si>
@@ -49,16 +49,63 @@
   </si>
   <si>
     <t>dob</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Kudi</t>
+  </si>
+  <si>
+    <t>google@gmail.com</t>
+  </si>
+  <si>
+    <t>65465564654</t>
+  </si>
+  <si>
+    <t>Sekdoid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,13 +128,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -366,15 +417,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -403,7 +455,116 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8456465</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>321</v>
+      </c>
+      <c r="H2">
+        <v>6545</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6954654654</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>624621</v>
+      </c>
+      <c r="H3">
+        <v>654654</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5464564</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>515</v>
+      </c>
+      <c r="H4">
+        <v>65454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6846546</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5">
+        <v>5154</v>
+      </c>
+      <c r="H5">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{627D3053-770C-455F-8293-EA1FBE8FFC88}"/>
+    <hyperlink ref="D3:D5" r:id="rId2" display="google@gmail.com" xr:uid="{BAD90928-7A5E-4DD2-ABE8-DB5856D5221F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>